<commit_message>
Creacion de .pix que permite las planillas de cualquier retailer, limpieza en los codigos de los principales retailers y cambio en la planilla base
</commit_message>
<xml_diff>
--- a/assets/plantilla de la planilla.xlsx
+++ b/assets/plantilla de la planilla.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d7475c5cd93efbfa/Desktop/BOTS/BOT 8 - Planilla y Despacho/Planilla_Despacho/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\autom\Desktop\BOTS\BOT 8 - Planilla y Despacho\Planilla_Despacho\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{E096A6DD-BE95-4CB5-88D2-B4F8C0CFEEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2D6A500-E5E1-4ED7-ABA8-83131128B46B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EBD6AF-9DC6-4AD9-8C58-F88A7C5237F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0894A5F1-6566-44AA-B290-C0243C5AEA2B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>FECHA</t>
   </si>
@@ -68,18 +68,6 @@
     <t>N° ORDEN</t>
   </si>
   <si>
-    <t>N° GUIA</t>
-  </si>
-  <si>
-    <t>COSTO</t>
-  </si>
-  <si>
-    <t>PRECIO SIN IVA</t>
-  </si>
-  <si>
-    <t>PRECIO CON IVA</t>
-  </si>
-  <si>
     <t>ITEM</t>
   </si>
   <si>
@@ -93,6 +81,9 @@
   </si>
   <si>
     <t>NO SE LLENA</t>
+  </si>
+  <si>
+    <t>FIRMA</t>
   </si>
 </sst>
 </file>
@@ -412,10 +403,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -735,52 +722,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01B00A5-36B9-4DCC-9213-74A1B670CC65}">
-  <dimension ref="B2:Q9"/>
+  <dimension ref="B2:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="12" width="18.109375" customWidth="1"/>
-    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" customWidth="1"/>
-    <col min="15" max="16" width="18.109375" customWidth="1"/>
+    <col min="2" max="13" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="17" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
     </row>
-    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="13"/>
       <c r="H4" s="14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="10" t="s">
-        <v>18</v>
+      <c r="L4" s="16"/>
+      <c r="M4" s="10" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:17" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:14" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -809,26 +790,17 @@
         <v>6</v>
       </c>
       <c r="K5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="P5" s="9" t="s">
+      <c r="M5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="Q5" s="2"/>
+      <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="2:17" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -841,12 +813,9 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="2"/>
+      <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -859,12 +828,9 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="2"/>
+      <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -876,13 +842,10 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="2"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -895,15 +858,12 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="2"/>
+      <c r="N9" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:O4"/>
+    <mergeCell ref="H4:L4"/>
     <mergeCell ref="B2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>